<commit_message>
test of multiple line of kv
</commit_message>
<xml_diff>
--- a/test/excels/test.xlsx
+++ b/test/excels/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B1C88C-DD01-4EDB-A091-FE85F42A149E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7288C21D-9807-499A-845F-F5C26CC39F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22268" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>this is a test file</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,6 +108,11 @@
   </si>
   <si>
     <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test {
+  "d1"  "d2" }</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -151,8 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -435,22 +443,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -488,7 +496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -514,7 +522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -527,6 +535,9 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
@@ -534,7 +545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -561,7 +572,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -573,9 +584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AB7083-F088-4BC4-9B33-9BD510AEDEEB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix a bug that caused by 0 == '' in javascript
</commit_message>
<xml_diff>
--- a/test/excels/test.xlsx
+++ b/test/excels/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F677AD52-37E9-4FE6-8AD8-8DDED767EA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9607AFBC-D71E-4FBE-BE66-98DEB4B91F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>this is a test file</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,6 +121,14 @@
   </si>
   <si>
     <t>测试key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  c  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -452,7 +460,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -526,6 +534,9 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
       <c r="K3" t="s">
         <v>8</v>
       </c>
@@ -549,6 +560,9 @@
       <c r="G4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
@@ -562,6 +576,9 @@
       </c>
       <c r="B5" t="s">
         <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
fixed the problem that #Loc interrupts simple kv file transpilation
</commit_message>
<xml_diff>
--- a/test/excels/test.xlsx
+++ b/test/excels/test.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9607AFBC-D71E-4FBE-BE66-98DEB4B91F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F538B72-4FF5-CA45-ADF0-F78E6D896E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1600" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="__Test" sheetId="3" r:id="rId3"/>
+    <sheet name="simple" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="__Test" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>this is a test file</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -129,6 +130,30 @@
   </si>
   <si>
     <t xml:space="preserve">  c  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Loc_Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -136,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,17 +484,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -515,7 +540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -544,7 +569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="32">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -570,7 +595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -598,12 +623,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F088BAA8-15C9-1346-A175-E01CEE802D36}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CCF6DB-2AC8-4D3F-8F08-08CC5E62BBE8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -611,13 +687,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AB7083-F088-4BC4-9B33-9BD510AEDEEB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>